<commit_message>
Version 1.2 adds support for PET/CBM MultiROM boards
PET/CBM Multi-ROM boards can be used in any 4K socket including the
Character ROM socket. This release adds support for padding with zeros
or duplicating 2K ROMs to make each entry 4K in size.
</commit_message>
<xml_diff>
--- a/MER-SET-01.xlsx
+++ b/MER-SET-01.xlsx
@@ -132,9 +132,6 @@
     <t>40</t>
   </si>
   <si>
-    <t>##</t>
-  </si>
-  <si>
     <t>COLS</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Multi-EditROM - SET #01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">you </t>
   </si>
 </sst>
 </file>
@@ -208,11 +208,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment textRotation="135"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -222,29 +224,10 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
           <bgColor theme="8" tint="0.39997558519241921"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="135" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="yyyy/mm/dd"/>
@@ -270,30 +253,50 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:O19" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:O19" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A3:O19"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="##" dataDxfId="2"/>
-    <tableColumn id="2" name="DIP" dataDxfId="0"/>
-    <tableColumn id="3" name="MODEL" dataDxfId="1"/>
+    <tableColumn id="1" name="you " dataDxfId="9"/>
+    <tableColumn id="2" name="DIP" dataDxfId="8"/>
+    <tableColumn id="3" name="MODEL" dataDxfId="7"/>
     <tableColumn id="4" name="KEYBRD"/>
-    <tableColumn id="5" name="IRQ" dataDxfId="9"/>
-    <tableColumn id="6" name="SCREEN" dataDxfId="8"/>
-    <tableColumn id="7" name="COLS" dataDxfId="7"/>
+    <tableColumn id="5" name="IRQ" dataDxfId="6"/>
+    <tableColumn id="6" name="SCREEN" dataDxfId="5"/>
+    <tableColumn id="7" name="COLS" dataDxfId="4"/>
     <tableColumn id="8" name="SOFT40"/>
-    <tableColumn id="9" name="SS 40/80" dataDxfId="6"/>
-    <tableColumn id="10" name="HARD 40/80" dataDxfId="5"/>
+    <tableColumn id="9" name="SS 40/80" dataDxfId="3"/>
+    <tableColumn id="10" name="HARD 40/80" dataDxfId="2"/>
     <tableColumn id="11" name="ESC"/>
     <tableColumn id="12" name="WEDGE"/>
     <tableColumn id="13" name="REBOOT"/>
     <tableColumn id="14" name="B-ARR"/>
-    <tableColumn id="15" name="DATE" dataDxfId="4"/>
+    <tableColumn id="15" name="DATE" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -589,86 +592,85 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="8.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" customWidth="1"/>
+    <col min="12" max="13" width="4.85546875" customWidth="1"/>
+    <col min="14" max="14" width="5.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.25">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="51">
+      <c r="A3" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2">
@@ -677,32 +679,32 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4">
-        <v>60</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="3">
+        <v>60</v>
+      </c>
+      <c r="F4" s="3">
         <v>20</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>40</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="N4" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="5">
+      <c r="O4" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2">
@@ -711,29 +713,29 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4">
-        <v>60</v>
-      </c>
-      <c r="F5" s="4">
+      <c r="E5" s="3">
+        <v>60</v>
+      </c>
+      <c r="F5" s="3">
         <v>20</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>40</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="O5" s="5">
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="O5" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2">
@@ -742,31 +744,31 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="4">
-        <v>60</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="3">
+        <v>60</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>80</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>80</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="3"/>
       <c r="N6" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="2">
@@ -775,32 +777,32 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4">
-        <v>60</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="3">
+        <v>60</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>40</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="N7" t="s">
         <v>30</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2">
@@ -809,19 +811,19 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="4">
-        <v>60</v>
-      </c>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>80</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>80</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="3"/>
       <c r="K8" t="s">
         <v>30</v>
       </c>
@@ -834,15 +836,15 @@
       <c r="N8" t="s">
         <v>30</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="4">
         <v>42797</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2">
@@ -851,19 +853,19 @@
       <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="4">
-        <v>60</v>
-      </c>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="3">
+        <v>60</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>80</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="4"/>
+      <c r="J9" s="3"/>
       <c r="K9" t="s">
         <v>30</v>
       </c>
@@ -876,15 +878,15 @@
       <c r="N9" t="s">
         <v>30</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2">
@@ -893,19 +895,19 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4">
-        <v>60</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="E10" s="3">
+        <v>60</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>80</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J10" s="4"/>
+      <c r="J10" s="3"/>
       <c r="K10" t="s">
         <v>30</v>
       </c>
@@ -918,15 +920,15 @@
       <c r="N10" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="2">
@@ -935,19 +937,19 @@
       <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="4">
-        <v>60</v>
-      </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="3">
+        <v>60</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>80</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J11" s="4"/>
+      <c r="J11" s="3"/>
       <c r="K11" t="s">
         <v>30</v>
       </c>
@@ -960,15 +962,15 @@
       <c r="N11" t="s">
         <v>30</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2">
@@ -977,17 +979,17 @@
       <c r="D12" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="4">
-        <v>60</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="3">
+        <v>60</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>80</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="K12" t="s">
@@ -1002,15 +1004,15 @@
       <c r="N12" t="s">
         <v>30</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="2">
@@ -1019,17 +1021,17 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="4">
-        <v>60</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="3">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>80</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="K13" t="s">
@@ -1044,15 +1046,15 @@
       <c r="N13" t="s">
         <v>30</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="2">
@@ -1061,17 +1063,17 @@
       <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="4">
-        <v>60</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="E14" s="3">
+        <v>60</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>80</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4" t="s">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="K14" t="s">
@@ -1086,15 +1088,15 @@
       <c r="N14" t="s">
         <v>30</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2">
@@ -1103,17 +1105,17 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="4">
-        <v>60</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="3">
+        <v>60</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>80</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="K15" t="s">
@@ -1128,15 +1130,15 @@
       <c r="N15" t="s">
         <v>30</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O15" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1145,17 +1147,17 @@
       <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="4">
-        <v>60</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="E16" s="3">
+        <v>60</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>40</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
       <c r="K16" t="s">
         <v>30</v>
       </c>
@@ -1168,15 +1170,15 @@
       <c r="N16" t="s">
         <v>30</v>
       </c>
-      <c r="O16" s="5">
+      <c r="O16" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1185,17 +1187,17 @@
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="4">
-        <v>60</v>
-      </c>
-      <c r="F17" s="4" t="s">
+      <c r="E17" s="3">
+        <v>60</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>40</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
       <c r="K17" t="s">
         <v>30</v>
       </c>
@@ -1208,15 +1210,15 @@
       <c r="N17" t="s">
         <v>30</v>
       </c>
-      <c r="O17" s="5">
+      <c r="O17" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1225,17 +1227,17 @@
       <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="4">
-        <v>60</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="3">
+        <v>60</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>40</v>
       </c>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
       <c r="K18" t="s">
         <v>30</v>
       </c>
@@ -1248,15 +1250,15 @@
       <c r="N18" t="s">
         <v>30</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="4">
         <v>42999</v>
       </c>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1265,17 +1267,17 @@
       <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="4">
-        <v>60</v>
-      </c>
-      <c r="F19" s="4" t="s">
+      <c r="E19" s="3">
+        <v>60</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>40</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
       <c r="K19" t="s">
         <v>30</v>
       </c>
@@ -1288,13 +1290,13 @@
       <c r="N19" t="s">
         <v>30</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <v>42999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="91" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>